<commit_message>
213,226 - Recent Estimation Schema and API
</commit_message>
<xml_diff>
--- a/Presentation/EstimationTool-Tables.xlsx
+++ b/Presentation/EstimationTool-Tables.xlsx
@@ -1132,8 +1132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>